<commit_message>
decision tree e dataset
</commit_message>
<xml_diff>
--- a/coding/dataset/dataset.xlsx
+++ b/coding/dataset/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomosanti/Documents/GitHub/ChallengeNao24/coding/dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiade\OneDrive\Desktop\nao24-github\ChallengeNao24\coding\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125621E2-B5DD-3842-8DAD-95E51AD1DF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34915F03-CF34-40F5-895F-2C91658F3F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="960" windowWidth="29400" windowHeight="17140" xr2:uid="{DEBDBBB0-A486-E642-A06E-38860BF9CAB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DEBDBBB0-A486-E642-A06E-38860BF9CAB5}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="176">
   <si>
     <t>angelic_bracelet</t>
   </si>
@@ -478,9 +478,6 @@
     <t>creativity_pendant</t>
   </si>
   <si>
-    <t>reativity pendant</t>
-  </si>
-  <si>
     <t>White, Rose gold-tone plated</t>
   </si>
   <si>
@@ -565,14 +562,14 @@
     <t>similar product_2</t>
   </si>
   <si>
-    <t>cambia</t>
+    <t>creativity pendant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -644,12 +641,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -663,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD883FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -873,72 +870,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -961,6 +938,26 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -986,9 +983,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1026,7 +1023,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1132,7 +1129,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1274,7 +1271,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1284,25 +1281,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B69ED41-DE86-7444-9225-823580E4F5E3}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="190" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="99" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="59.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="53.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="34.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" style="1"/>
+    <col min="6" max="6" width="59.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.796875" style="1"/>
+    <col min="9" max="9" width="53.69921875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.296875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="7" t="s">
         <v>125</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="20" customFormat="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1366,519 +1363,519 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+    <row r="3" spans="1:10" s="20" customFormat="1">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="26">
         <v>230</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
+    <row r="4" spans="1:10" s="20" customFormat="1">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>135</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="19" t="s">
+      <c r="G4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="20" customFormat="1">
       <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="17">
         <v>145</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="22" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18">
+    <row r="6" spans="1:10" s="20" customFormat="1">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>155</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="19" t="s">
+      <c r="G6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18">
+    <row r="7" spans="1:10" s="20" customFormat="1">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="17">
         <v>155</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
+    <row r="8" spans="1:10" s="20" customFormat="1">
+      <c r="A8" s="38">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="40">
         <v>155</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="G8" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18">
+    <row r="9" spans="1:10" s="20" customFormat="1">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="22">
         <v>175</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="20" customFormat="1">
       <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="17">
         <v>175</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="19" t="s">
+      <c r="G10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="22" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18">
+    <row r="11" spans="1:10" s="20" customFormat="1">
+      <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="17">
         <v>195</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27">
+    <row r="12" spans="1:10" s="20" customFormat="1">
+      <c r="A12" s="39">
         <v>11</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="43">
         <v>195</v>
       </c>
-      <c r="F12" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="15" t="s">
+      <c r="F12" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="J12" s="32" t="s">
+      <c r="J12" s="43" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18">
+    <row r="13" spans="1:10" s="20" customFormat="1">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="17">
         <v>195</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="19" t="s">
+      <c r="G13" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="22" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
+    <row r="14" spans="1:10" s="20" customFormat="1">
+      <c r="A14" s="25">
         <v>13</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="26">
         <v>195</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="G14" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="I14" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27">
+    <row r="15" spans="1:10" s="20" customFormat="1">
+      <c r="A15" s="39">
         <v>14</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="40">
         <v>250</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="G15" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="15" t="s">
+      <c r="G15" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="40" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="14">
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="22">
         <v>195</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="19" t="s">
+      <c r="G16" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="18">
+    <row r="17" spans="1:10">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="17">
         <v>125</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="19" t="s">
+      <c r="G17" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="18">
+    <row r="18" spans="1:10">
+      <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="17">
         <v>95</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="19" t="s">
+      <c r="G18" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1894,7 +1891,7 @@
       <c r="E19" s="6">
         <v>400</v>
       </c>
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="37" t="s">
         <v>41</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1910,7 +1907,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1942,7 +1939,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1974,7 +1971,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1990,7 +1987,7 @@
       <c r="E22" s="6">
         <v>135</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="37" t="s">
         <v>66</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -2006,39 +2003,39 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="27">
+    <row r="23" spans="1:10">
+      <c r="A23" s="39">
         <v>22</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="D23" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="E23" s="40">
+        <v>300</v>
+      </c>
+      <c r="F23" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="15">
-        <v>300</v>
-      </c>
-      <c r="F23" s="36" t="s">
+      <c r="G23" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I23" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="G23" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2070,7 +2067,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2102,7 +2099,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2134,7 +2131,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="15" customFormat="1">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2166,7 +2163,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="15" customFormat="1">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2198,7 +2195,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="15" customFormat="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" s="15" customFormat="1">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2262,7 +2259,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" s="15" customFormat="1">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2294,391 +2291,391 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B32" s="16" t="s">
+    <row r="32" spans="1:10" s="15" customFormat="1">
+      <c r="A32" s="39">
+        <v>36</v>
+      </c>
+      <c r="B32" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="E32" s="40">
+        <v>75</v>
+      </c>
+      <c r="F32" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="15">
-        <v>75</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H32" s="15" t="s">
+      <c r="G32" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I32" s="16" t="s">
+      <c r="I32" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="26">
+    <row r="33" spans="1:10" s="15" customFormat="1">
+      <c r="A33" s="38">
         <v>31</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="E33" s="40">
+        <v>125</v>
+      </c>
+      <c r="F33" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="J33" s="40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="15" customFormat="1">
+      <c r="A34" s="38">
+        <v>42</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="40">
+        <v>400</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="J34" s="40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="15" customFormat="1">
+      <c r="A35" s="39">
+        <v>39</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="40">
+        <v>230</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I35" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="15" customFormat="1">
+      <c r="A36" s="38">
+        <v>32</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="40">
+        <v>215</v>
+      </c>
+      <c r="F36" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="J36" s="40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="15" customFormat="1">
+      <c r="A37" s="39">
+        <v>40</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="40">
+        <v>250</v>
+      </c>
+      <c r="F37" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I37" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="J37" s="40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="15" customFormat="1">
+      <c r="A38" s="38">
+        <v>33</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="40">
+        <v>300</v>
+      </c>
+      <c r="F38" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G38" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="J38" s="40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="15" customFormat="1">
+      <c r="A39" s="39">
+        <v>41</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="40">
+        <v>175</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I39" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" s="40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="15" customFormat="1">
+      <c r="A40" s="38">
+        <v>38</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" s="40">
+        <v>175</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="J40" s="40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="15" customFormat="1">
+      <c r="A41" s="39">
         <v>34</v>
       </c>
-      <c r="D33" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E33" s="15">
-        <v>125</v>
-      </c>
-      <c r="F33" s="16" t="s">
+      <c r="B41" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="40">
+        <v>89</v>
+      </c>
+      <c r="F41" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="G33" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="I33" s="16" t="s">
+      <c r="G41" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I41" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="J41" s="40" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C34" s="15" t="s">
+    <row r="42" spans="1:10" s="15" customFormat="1">
+      <c r="A42" s="38">
+        <v>37</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="40">
+        <v>550</v>
+      </c>
+      <c r="F42" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="J42" s="40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="15" customFormat="1">
+      <c r="A43" s="39">
         <v>35</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E34" s="15">
-        <v>400</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="E35" s="15">
-        <v>230</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E36" s="15">
-        <v>215</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="15" t="s">
+      <c r="B43" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="E43" s="40">
+        <v>175</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I36" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E37" s="15">
-        <v>250</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="15">
-        <v>300</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I38" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" s="15">
-        <v>175</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E40" s="15">
-        <v>175</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" s="15">
-        <v>89</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="J41" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="15">
-        <v>550</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" s="15">
-        <v>175</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="J43" s="15" t="s">
+      <c r="J43" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" s="15" customFormat="1">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -2690,40 +2687,40 @@
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="B45" s="39"/>
-    </row>
-    <row r="46" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="11" customFormat="1">
+      <c r="A45" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="29"/>
+    </row>
+    <row r="46" spans="1:10" s="11" customFormat="1">
       <c r="A46" s="12"/>
       <c r="B46" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="11" customFormat="1">
+      <c r="A47" s="47"/>
+      <c r="B47" s="11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="28"/>
-      <c r="B47" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" s="11" customFormat="1">
       <c r="A48" s="13"/>
       <c r="B48" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="11" customFormat="1">
+      <c r="A49" s="24"/>
+      <c r="B49" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
-      <c r="B49" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:2" s="11" customFormat="1"/>
+    <row r="51" spans="1:2" s="11" customFormat="1"/>
+    <row r="52" spans="1:2" s="11" customFormat="1"/>
+    <row r="53" spans="1:2" s="11" customFormat="1"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J43">
     <sortCondition ref="A2:A43"/>
@@ -2741,202 +2738,202 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.1640625" customWidth="1"/>
+    <col min="1" max="1" width="35.796875" customWidth="1"/>
+    <col min="2" max="2" width="59.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="41"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="B3" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="41"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="C4" s="31"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="40" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="41"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="C6" s="31"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="41"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="C7" s="31"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="40"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="C8" s="30"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="42"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="19" t="s">
+      <c r="C9" s="32"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="C11" s="19" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" s="19" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="B13" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="41"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="C15" s="31"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="41"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="C16" s="31"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>150</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="B17" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="B19" s="44" t="s">
+      <c r="B18" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="44"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="43"/>
+      <c r="C19" s="34"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="33"/>
       <c r="B20" s="10"/>
     </row>
   </sheetData>

</xml_diff>